<commit_message>
Added JMeter tests and results
</commit_message>
<xml_diff>
--- a/TermProject/CS296N-TermProjectProposalRubric.xlsx
+++ b/TermProject/CS296N-TermProjectProposalRubric.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CS296N-CourseMaterials\TermProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS296N-CourseMaterials/TermProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF8D7C1-A95F-44A7-96D2-6493378D6803}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BEC98E-14FE-8349-B992-7DA05E2DD68C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3324" yWindow="576" windowWidth="8076" windowHeight="15900" xr2:uid="{316ADB5B-05A5-4789-A423-CE5C922A4BC8}"/>
+    <workbookView xWindow="3320" yWindow="500" windowWidth="10000" windowHeight="14600" activeTab="1" xr2:uid="{316ADB5B-05A5-4789-A423-CE5C922A4BC8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rubric" sheetId="1" r:id="rId1"/>
+    <sheet name="Grading" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Term Project Proposal Rubric</t>
   </si>
@@ -61,14 +53,37 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     10 to 15 pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     4 to 6 classes, 12 to 30 fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     rich media, data, authorization</t>
+  </si>
+  <si>
+    <t>No diagram</t>
+  </si>
+  <si>
+    <t>minimal detail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -96,8 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,34 +429,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848E1DFE-844E-4152-84AD-3F406D8D810D}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B4:B10)</f>
+        <v>50</v>
+      </c>
+      <c r="C12">
+        <f>SUM(C4:C10)</f>
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA0A454-2F82-334C-833A-4427ED2ECD89}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A3" sqref="A3:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -449,8 +573,12 @@
       <c r="C4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F6" si="0">C4/B4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -458,10 +586,17 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -471,8 +606,12 @@
       <c r="C6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -480,11 +619,21 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2">
+        <f>C7/B7</f>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -493,7 +642,11 @@
       </c>
       <c r="C9">
         <f>SUM(C4:C7)</f>
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" ref="F9" si="1">C9/B9</f>
+        <v>0.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>